<commit_message>
Admin and Manager login modules feature files
</commit_message>
<xml_diff>
--- a/TestData/Excel_data/Stratos_Test_Data.xlsx
+++ b/TestData/Excel_data/Stratos_Test_Data.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B073FD93-D195-4F4C-A2E5-7C1B05574B56}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6C847520-4E53-4428-9B2F-468181D1AE5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15410" windowHeight="1570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13960" windowHeight="5730" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOGIN" sheetId="1" r:id="rId1"/>
+    <sheet name="3RD PARTY PROVIDER" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:I18"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Username</t>
   </si>
@@ -33,6 +34,69 @@
   </si>
   <si>
     <t>sam123@gmail.com</t>
+  </si>
+  <si>
+    <t>Provider Name</t>
+  </si>
+  <si>
+    <t>Mobile Number</t>
+  </si>
+  <si>
+    <t>Other Contact Number</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saran </t>
+  </si>
+  <si>
+    <t>Fax Number</t>
+  </si>
+  <si>
+    <t>Vat Number</t>
+  </si>
+  <si>
+    <t>27832GAF*&amp;</t>
+  </si>
+  <si>
+    <t>87378HS&amp;$#</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>Street2</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>97483HSF%#</t>
+  </si>
+  <si>
+    <t>8727GTH&amp;^%</t>
+  </si>
+  <si>
+    <t>saran@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -363,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -404,4 +468,102 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6650E07E-7075-45BE-BA25-ACC8F76A0F46}">
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{815B796C-F77A-414D-ACD5-68C626234956}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated provider glue code
</commit_message>
<xml_diff>
--- a/TestData/Excel_data/Stratos_Test_Data.xlsx
+++ b/TestData/Excel_data/Stratos_Test_Data.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6C847520-4E53-4428-9B2F-468181D1AE5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{23EFFAF6-082B-46C3-A071-6EA23C595ED3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13960" windowHeight="5730" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="5730" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOGIN" sheetId="1" r:id="rId1"/>
     <sheet name="3RD PARTY PROVIDER" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I18"/>
+  <oleSize ref="A1:K18"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Username</t>
   </si>
@@ -48,21 +48,12 @@
     <t>Email Address</t>
   </si>
   <si>
-    <t xml:space="preserve">Saran </t>
-  </si>
-  <si>
     <t>Fax Number</t>
   </si>
   <si>
     <t>Vat Number</t>
   </si>
   <si>
-    <t>27832GAF*&amp;</t>
-  </si>
-  <si>
-    <t>87378HS&amp;$#</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -90,20 +81,38 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>97483HSF%#</t>
-  </si>
-  <si>
-    <t>8727GTH&amp;^%</t>
-  </si>
-  <si>
-    <t>saran@gmail.com</t>
+    <t>Justice Mahomed St &amp; Steve Biko streets, Sunnyside, Pretoria, 0001, South Africa</t>
+  </si>
+  <si>
+    <t>xyz@gmail.com</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>Pretoria</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Gauteng</t>
+  </si>
+  <si>
+    <t>This is to create sample provider</t>
+  </si>
+  <si>
+    <t>959 Arcadia Street Hatfield, Pretoria, 0001, South Africa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +127,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF19344E"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,9 +156,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -428,7 +451,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -472,96 +495,116 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6650E07E-7075-45BE-BA25-ACC8F76A0F46}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="8.7265625" style="3"/>
+    <col min="13" max="13" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.81640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="3">
+        <v>9984738816</v>
+      </c>
+      <c r="C2" s="3">
+        <v>8972736635</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="3">
+        <v>7782937352</v>
+      </c>
+      <c r="F2" s="3">
+        <v>9973263547</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" t="s">
-        <v>21</v>
+      <c r="I2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="5">
+        <v>1111</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{815B796C-F77A-414D-ACD5-68C626234956}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{A829F1DA-5966-4FF1-BD94-CE57DEA3D97E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Commiting Employee and ACL Users glue code
</commit_message>
<xml_diff>
--- a/TestData/Excel_data/Stratos_Test_Data.xlsx
+++ b/TestData/Excel_data/Stratos_Test_Data.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{23EFFAF6-082B-46C3-A071-6EA23C595ED3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{72F769CD-33A4-4E11-AE96-2D93E146A6FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="5730" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13940" windowHeight="1730" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOGIN" sheetId="1" r:id="rId1"/>
     <sheet name="3RD PARTY PROVIDER" sheetId="2" r:id="rId2"/>
+    <sheet name="Manage ACL Users" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K18"/>
+  <oleSize ref="A1:N18"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Username</t>
   </si>
@@ -84,12 +85,6 @@
     <t>Justice Mahomed St &amp; Steve Biko streets, Sunnyside, Pretoria, 0001, South Africa</t>
   </si>
   <si>
-    <t>xyz@gmail.com</t>
-  </si>
-  <si>
-    <t>xyz</t>
-  </si>
-  <si>
     <t>Pretoria</t>
   </si>
   <si>
@@ -103,6 +98,36 @@
   </si>
   <si>
     <t>959 Arcadia Street Hatfield, Pretoria, 0001, South Africa</t>
+  </si>
+  <si>
+    <t>Filter Data</t>
+  </si>
+  <si>
+    <t>Amchi pvt lmd</t>
+  </si>
+  <si>
+    <t>sample-008</t>
+  </si>
+  <si>
+    <t>sample.008@gmail.com</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>Saran</t>
+  </si>
+  <si>
+    <t>saran@gmail.com</t>
+  </si>
+  <si>
+    <t>Saga</t>
   </si>
 </sst>
 </file>
@@ -156,7 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -167,6 +192,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -495,10 +523,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6650E07E-7075-45BE-BA25-ACC8F76A0F46}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -512,9 +540,12 @@
     <col min="7" max="12" width="8.7265625" style="3"/>
     <col min="13" max="13" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7265625" style="8" customWidth="1"/>
+    <col min="16" max="16" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -557,10 +588,15 @@
       <c r="N1" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="O1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3">
         <v>9984738816</v>
@@ -568,8 +604,8 @@
       <c r="C2" s="3">
         <v>8972736635</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>20</v>
+      <c r="D2" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="E2" s="3">
         <v>7782937352</v>
@@ -584,22 +620,25 @@
         <v>19</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="L2" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M2" s="5">
         <v>1111</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -609,4 +648,71 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DF39FE6-F612-4CC4-BCA6-A06A7C96E1EC}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2">
+        <v>111111</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2">
+        <v>9987635263</v>
+      </c>
+      <c r="F2">
+        <v>111111</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{F0963025-2590-4EFB-900D-C2F8BCAA89FE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>